<commit_message>
Adjust crop_target for axis offset
</commit_message>
<xml_diff>
--- a/evaluation/Versuchsplan.xlsx
+++ b/evaluation/Versuchsplan.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="61">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t xml:space="preserve">ZED2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20°</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40°</t>
   </si>
   <si>
     <t xml:space="preserve">Lighting (bright/dark)</t>
@@ -238,18 +244,12 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3715A"/>
-        <bgColor rgb="FFFF6600"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -286,7 +286,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -299,10 +299,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -312,66 +308,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFF3715A"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -1680,10 +1616,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1695,7 +1631,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1722,27 +1658,34 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
-        <v>12</v>
+      <c r="C2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
+      <c r="A3" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>54</v>
@@ -1751,7 +1694,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>360</v>
@@ -1767,29 +1710,34 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3" t="s">
-        <v>12</v>
+      <c r="C4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
+      <c r="A5" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>54</v>
@@ -1798,7 +1746,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>360</v>
@@ -1814,29 +1762,34 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3" t="s">
-        <v>12</v>
+      <c r="C6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>17</v>
+      <c r="A7" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>54</v>
@@ -1845,471 +1798,204 @@
         <v>10</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="0" t="n">
         <v>360</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="3" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3" t="s">
-        <v>12</v>
+      <c r="G8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>19</v>
+      <c r="A9" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>360</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>51</v>
-      </c>
       <c r="G9" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="H9" s="0" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="3" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3" t="s">
-        <v>12</v>
+      <c r="C10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>21</v>
+      <c r="A11" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>360</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="H11" s="0" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
+      <c r="A12" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>360</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="H12" s="0" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3" t="s">
-        <v>12</v>
+      <c r="C13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>26</v>
+      <c r="A14" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>11</v>
+        <v>2</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>360</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>12</v>
+        <v>56</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="3" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="0" t="n">
+      <c r="C15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E16" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="3" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="3" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="3" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G28" s="0" t="s">
+      <c r="E15" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="G15" s="0" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
+      <c r="H15" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A:H"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2356,7 +2042,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>6</v>
@@ -2370,7 +2056,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>10</v>
@@ -2390,7 +2076,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>10</v>
@@ -2410,7 +2096,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>10</v>
@@ -2430,7 +2116,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>10</v>
@@ -2450,7 +2136,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>10</v>
@@ -2470,7 +2156,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>10</v>
@@ -2490,7 +2176,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>10</v>
@@ -2510,7 +2196,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>10</v>
@@ -2530,7 +2216,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>10</v>
@@ -2550,7 +2236,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>10</v>
@@ -2570,7 +2256,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>10</v>
@@ -2590,7 +2276,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>25</v>
@@ -2610,7 +2296,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>25</v>
@@ -2630,7 +2316,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>25</v>
@@ -2650,7 +2336,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>25</v>
@@ -2670,7 +2356,7 @@
         <v>29</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>25</v>
@@ -2690,7 +2376,7 @@
         <v>30</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>25</v>
@@ -2710,7 +2396,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>25</v>
@@ -2730,7 +2416,7 @@
         <v>32</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>25</v>
@@ -2750,7 +2436,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>25</v>
@@ -2770,7 +2456,7 @@
         <v>34</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>25</v>
@@ -2790,7 +2476,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>25</v>
@@ -2810,7 +2496,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>37</v>
@@ -2830,7 +2516,7 @@
         <v>39</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>10</v>
@@ -2850,7 +2536,7 @@
         <v>41</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>10</v>
@@ -2870,7 +2556,7 @@
         <v>43</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>10</v>
@@ -2890,7 +2576,7 @@
         <v>45</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>10</v>
@@ -2910,7 +2596,7 @@
         <v>47</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>10</v>
@@ -2969,7 +2655,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>6</v>
@@ -2983,7 +2669,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>10</v>
@@ -3003,7 +2689,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>10</v>
@@ -3023,7 +2709,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>10</v>
@@ -3043,7 +2729,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>10</v>
@@ -3063,7 +2749,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>10</v>
@@ -3083,7 +2769,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>10</v>
@@ -3103,7 +2789,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>10</v>
@@ -3123,7 +2809,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>10</v>
@@ -3143,7 +2829,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>10</v>
@@ -3163,7 +2849,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>10</v>
@@ -3183,7 +2869,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>10</v>
@@ -3203,7 +2889,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>25</v>
@@ -3223,7 +2909,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>25</v>
@@ -3243,7 +2929,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>25</v>
@@ -3263,7 +2949,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>25</v>
@@ -3283,7 +2969,7 @@
         <v>29</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>25</v>
@@ -3303,7 +2989,7 @@
         <v>30</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>25</v>
@@ -3323,7 +3009,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>25</v>
@@ -3343,7 +3029,7 @@
         <v>32</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>25</v>
@@ -3363,7 +3049,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>25</v>
@@ -3383,7 +3069,7 @@
         <v>34</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>25</v>
@@ -3403,7 +3089,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>25</v>
@@ -3423,7 +3109,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>37</v>
@@ -3443,7 +3129,7 @@
         <v>39</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>10</v>
@@ -3463,7 +3149,7 @@
         <v>41</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>10</v>
@@ -3483,7 +3169,7 @@
         <v>43</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>10</v>
@@ -3503,7 +3189,7 @@
         <v>45</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>10</v>
@@ -3523,7 +3209,7 @@
         <v>47</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>10</v>
@@ -3582,7 +3268,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>6</v>
@@ -3596,7 +3282,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>10</v>
@@ -3616,7 +3302,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>10</v>
@@ -3636,7 +3322,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>10</v>
@@ -3656,7 +3342,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>10</v>
@@ -3676,7 +3362,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>10</v>
@@ -3696,7 +3382,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>10</v>
@@ -3716,7 +3402,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>10</v>
@@ -3736,7 +3422,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>10</v>
@@ -3756,7 +3442,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>10</v>
@@ -3776,7 +3462,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>10</v>
@@ -3796,7 +3482,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>10</v>
@@ -3816,7 +3502,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>25</v>
@@ -3836,7 +3522,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>25</v>
@@ -3856,7 +3542,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>25</v>
@@ -3876,7 +3562,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>25</v>
@@ -3896,7 +3582,7 @@
         <v>29</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>25</v>
@@ -3916,7 +3602,7 @@
         <v>30</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>25</v>
@@ -3936,7 +3622,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>25</v>
@@ -3956,7 +3642,7 @@
         <v>32</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>25</v>
@@ -3976,7 +3662,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>25</v>
@@ -3996,7 +3682,7 @@
         <v>34</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>25</v>
@@ -4016,7 +3702,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>25</v>
@@ -4036,7 +3722,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>37</v>
@@ -4056,7 +3742,7 @@
         <v>39</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>10</v>
@@ -4076,7 +3762,7 @@
         <v>41</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>10</v>
@@ -4096,7 +3782,7 @@
         <v>43</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>10</v>
@@ -4116,7 +3802,7 @@
         <v>45</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>10</v>
@@ -4136,7 +3822,7 @@
         <v>47</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
update orbbec and realsense
</commit_message>
<xml_diff>
--- a/evaluation/Versuchsplan.xlsx
+++ b/evaluation/Versuchsplan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="D435" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="35">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
@@ -54,7 +54,19 @@
     <t xml:space="preserve">Done</t>
   </si>
   <si>
-    <t xml:space="preserve">01</t>
+    <t xml:space="preserve">Bias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edge Precision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sphere</t>
   </si>
   <si>
     <t xml:space="preserve">D435</t>
@@ -72,75 +84,39 @@
     <t xml:space="preserve">x</t>
   </si>
   <si>
-    <t xml:space="preserve">Offset Rangefinder -&gt; Camera: -20mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07</t>
-  </si>
-  <si>
     <t xml:space="preserve">sphere</t>
   </si>
   <si>
-    <t xml:space="preserve">08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
     <t xml:space="preserve">rect shiny</t>
   </si>
   <si>
-    <t xml:space="preserve">12</t>
-  </si>
-  <si>
     <t xml:space="preserve">20°</t>
   </si>
   <si>
-    <t xml:space="preserve">13</t>
-  </si>
-  <si>
     <t xml:space="preserve">40°</t>
   </si>
   <si>
-    <t xml:space="preserve">14</t>
-  </si>
-  <si>
     <t xml:space="preserve">60°</t>
   </si>
   <si>
+    <t xml:space="preserve">Offset Rangefinder -&gt; Camera: -10mm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Distance rangefinder [m]</t>
   </si>
   <si>
     <t xml:space="preserve">D455</t>
   </si>
   <si>
+    <t xml:space="preserve">Offset Rangefinder -&gt; Camera: -12mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZED2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Offset Rangefinder -&gt; Camera: -15mm</t>
   </si>
   <si>
-    <t xml:space="preserve">ZED2</t>
-  </si>
-  <si>
     <t xml:space="preserve">OAK-D</t>
   </si>
   <si>
@@ -148,6 +124,15 @@
   </si>
   <si>
     <t xml:space="preserve">Astra Stereo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1280*800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">failed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offset Rangefinder -&gt; Camera: -35mm</t>
   </si>
 </sst>
 </file>
@@ -157,12 +142,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -179,135 +165,16 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
-    <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -315,23 +182,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -355,57 +207,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -421,91 +222,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -518,10 +242,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -532,7 +256,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -557,16 +281,31 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
+      <c r="A2" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -575,27 +314,24 @@
         <v>360</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H2" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>2</v>
@@ -604,24 +340,24 @@
         <v>360</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H3" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>3</v>
@@ -630,24 +366,24 @@
         <v>360</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H4" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>4</v>
@@ -656,24 +392,24 @@
         <v>360</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H5" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>5</v>
@@ -682,24 +418,24 @@
         <v>360</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H6" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="C7" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>2</v>
@@ -708,24 +444,24 @@
         <v>30</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H7" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="C8" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -734,50 +470,50 @@
         <v>360</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H8" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="C9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>360</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="0" t="s">
+      <c r="B10" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="C10" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>3</v>
@@ -786,24 +522,24 @@
         <v>360</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H10" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="C11" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>2</v>
@@ -812,76 +548,76 @@
         <v>30</v>
       </c>
       <c r="F11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="B12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="B13" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>360</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="0" t="s">
+      <c r="C13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>360</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="0" t="s">
+      <c r="B14" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="C14" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>2</v>
@@ -890,24 +626,24 @@
         <v>360</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="H14" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="C15" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>2</v>
@@ -916,16 +652,21 @@
         <v>360</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -956,10 +697,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1048576"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -971,7 +712,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -982,7 +723,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>4</v>
@@ -996,16 +737,31 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
+      <c r="A2" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -1014,27 +770,24 @@
         <v>360</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>15</v>
+      <c r="A3" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>2</v>
@@ -1043,24 +796,24 @@
         <v>360</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
+      <c r="A4" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>3</v>
@@ -1069,24 +822,24 @@
         <v>360</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
+      <c r="A5" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>4</v>
@@ -1095,24 +848,24 @@
         <v>360</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
+      <c r="A6" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>5</v>
@@ -1121,24 +874,24 @@
         <v>360</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
+      <c r="A7" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>2</v>
@@ -1147,24 +900,24 @@
         <v>30</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
+      <c r="A8" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -1173,24 +926,24 @@
         <v>360</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
+      <c r="A9" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>2</v>
@@ -1199,24 +952,24 @@
         <v>360</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
+      <c r="A10" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>3</v>
@@ -1225,24 +978,24 @@
         <v>360</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
+      <c r="A11" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>2</v>
@@ -1251,105 +1004,122 @@
         <v>30</v>
       </c>
       <c r="F11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="B12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="B13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="B14" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="0" t="s">
+      <c r="C14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>360</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>360</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>360</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>360</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1382,10 +1152,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1048576"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1394,7 +1164,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="7" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1422,16 +1194,31 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -1440,16 +1227,10 @@
         <v>360</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1457,10 +1238,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>2</v>
@@ -1469,13 +1250,10 @@
         <v>360</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1483,10 +1261,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>3</v>
@@ -1495,13 +1273,10 @@
         <v>360</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1509,10 +1284,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>4</v>
@@ -1521,13 +1296,10 @@
         <v>360</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1535,10 +1307,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>5</v>
@@ -1547,13 +1319,10 @@
         <v>360</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1561,10 +1330,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>2</v>
@@ -1573,13 +1342,10 @@
         <v>30</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1587,10 +1353,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -1599,13 +1365,10 @@
         <v>360</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1613,10 +1376,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>2</v>
@@ -1625,13 +1388,10 @@
         <v>360</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1639,10 +1399,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>3</v>
@@ -1651,13 +1411,10 @@
         <v>360</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1665,10 +1422,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>2</v>
@@ -1677,13 +1434,10 @@
         <v>30</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1691,10 +1445,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>2</v>
@@ -1703,13 +1457,10 @@
         <v>360</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1717,10 +1468,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>2</v>
@@ -1729,13 +1480,10 @@
         <v>360</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1743,10 +1491,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>2</v>
@@ -1755,13 +1503,10 @@
         <v>360</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1769,10 +1514,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>2</v>
@@ -1781,13 +1526,15 @@
         <v>360</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>13</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1810,10 +1557,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1847,16 +1594,34 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
+      <c r="A2" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -1865,21 +1630,21 @@
         <v>360</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>15</v>
+      <c r="A3" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>2</v>
@@ -1888,21 +1653,21 @@
         <v>360</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
+      <c r="A4" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>3</v>
@@ -1911,21 +1676,21 @@
         <v>360</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
+      <c r="A5" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>4</v>
@@ -1934,21 +1699,21 @@
         <v>360</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
+      <c r="A6" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>5</v>
@@ -1957,21 +1722,21 @@
         <v>360</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
+      <c r="A7" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>2</v>
@@ -1980,21 +1745,21 @@
         <v>30</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
+      <c r="A8" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -2003,21 +1768,21 @@
         <v>360</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
+      <c r="A9" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>2</v>
@@ -2026,21 +1791,21 @@
         <v>360</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
+      <c r="A10" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>3</v>
@@ -2049,21 +1814,21 @@
         <v>360</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
+      <c r="A11" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>2</v>
@@ -2072,44 +1837,44 @@
         <v>30</v>
       </c>
       <c r="F11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="B12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>360</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="B13" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>2</v>
@@ -2118,21 +1883,21 @@
         <v>360</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>37</v>
-      </c>
       <c r="C14" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>2</v>
@@ -2141,21 +1906,21 @@
         <v>360</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>31</v>
+      <c r="A15" s="1" t="n">
+        <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>2</v>
@@ -2164,10 +1929,10 @@
         <v>360</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2200,10 +1965,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2237,16 +2002,34 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
+      <c r="A2" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -2255,21 +2038,21 @@
         <v>360</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>15</v>
+      <c r="A3" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>2</v>
@@ -2278,21 +2061,21 @@
         <v>360</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
+      <c r="A4" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>3</v>
@@ -2301,21 +2084,21 @@
         <v>360</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
+      <c r="A5" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>4</v>
@@ -2324,21 +2107,21 @@
         <v>360</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
+      <c r="A6" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>5</v>
@@ -2347,21 +2130,21 @@
         <v>360</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
+      <c r="A7" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>2</v>
@@ -2370,21 +2153,21 @@
         <v>30</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
+      <c r="A8" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -2393,21 +2176,21 @@
         <v>360</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
+      <c r="A9" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>2</v>
@@ -2416,21 +2199,21 @@
         <v>360</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
+      <c r="A10" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>3</v>
@@ -2439,21 +2222,21 @@
         <v>360</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
+      <c r="A11" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>2</v>
@@ -2462,44 +2245,44 @@
         <v>30</v>
       </c>
       <c r="F11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="B12" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>360</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="B13" s="0" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>2</v>
@@ -2508,21 +2291,21 @@
         <v>360</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>29</v>
+      <c r="A14" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>2</v>
@@ -2531,21 +2314,21 @@
         <v>360</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G14" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="C15" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>2</v>
@@ -2554,10 +2337,10 @@
         <v>360</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2590,10 +2373,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2627,16 +2410,34 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
+      <c r="A2" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -2645,21 +2446,24 @@
         <v>360</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>15</v>
+      <c r="A3" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>2</v>
@@ -2668,21 +2472,24 @@
         <v>360</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
+      <c r="A4" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>3</v>
@@ -2691,21 +2498,24 @@
         <v>360</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
+      <c r="A5" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>4</v>
@@ -2714,21 +2524,24 @@
         <v>360</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
+      <c r="A6" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>5</v>
@@ -2737,21 +2550,24 @@
         <v>360</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
+      <c r="A7" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>2</v>
@@ -2760,21 +2576,24 @@
         <v>30</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
+      <c r="A8" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -2783,21 +2602,24 @@
         <v>360</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
+      <c r="A9" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>2</v>
@@ -2806,21 +2628,24 @@
         <v>360</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
+      <c r="A10" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>3</v>
@@ -2829,21 +2654,24 @@
         <v>360</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
+      <c r="A11" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>2</v>
@@ -2852,44 +2680,50 @@
         <v>30</v>
       </c>
       <c r="F11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="B12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>360</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="B13" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>2</v>
@@ -2898,21 +2732,24 @@
         <v>360</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>29</v>
+      <c r="A14" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>2</v>
@@ -2921,21 +2758,24 @@
         <v>360</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>30</v>
+        <v>21</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="C15" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>2</v>
@@ -2944,10 +2784,18 @@
         <v>360</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
update bias calc for no edges
</commit_message>
<xml_diff>
--- a/evaluation/Versuchsplan.xlsx
+++ b/evaluation/Versuchsplan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="D435" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="40">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
@@ -103,6 +103,21 @@
   </si>
   <si>
     <t xml:space="preserve">Distance rangefinder [m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NaN-Ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edge left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edge down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edge right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edge up</t>
   </si>
   <si>
     <t xml:space="preserve">D455</t>
@@ -244,7 +259,7 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -697,19 +712,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="33.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="7" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="20.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -744,12 +761,24 @@
         <v>9</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="L1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="Q1" s="0" t="s">
         <v>12</v>
       </c>
     </row>
@@ -758,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>14</v>
@@ -778,13 +807,34 @@
       <c r="H2" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="I2" s="0" t="n">
+        <v>0.00452</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>0.00528</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>0.00048</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>1.75261</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>0.83784</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>0.78911</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>1.62116</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>14</v>
@@ -803,6 +853,27 @@
       </c>
       <c r="H3" s="0" t="s">
         <v>17</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0.01079</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0.00237</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>3.20879</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>4.44525</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>2.79416</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>1.75754</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,7 +881,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>14</v>
@@ -836,7 +907,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>14</v>
@@ -862,7 +933,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>14</v>
@@ -888,7 +959,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>14</v>
@@ -914,7 +985,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>18</v>
@@ -940,7 +1011,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>18</v>
@@ -966,7 +1037,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>18</v>
@@ -992,7 +1063,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>18</v>
@@ -1018,7 +1089,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>19</v>
@@ -1044,7 +1115,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>14</v>
@@ -1070,7 +1141,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>14</v>
@@ -1096,7 +1167,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>14</v>
@@ -1119,23 +1190,9 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1154,7 +1211,7 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1215,7 +1272,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>14</v>
@@ -1238,7 +1295,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>14</v>
@@ -1261,7 +1318,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>14</v>
@@ -1284,7 +1341,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>14</v>
@@ -1307,7 +1364,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>14</v>
@@ -1330,7 +1387,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>14</v>
@@ -1353,7 +1410,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>18</v>
@@ -1376,7 +1433,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>18</v>
@@ -1399,7 +1456,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>18</v>
@@ -1422,7 +1479,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>18</v>
@@ -1445,7 +1502,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>19</v>
@@ -1468,7 +1525,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>14</v>
@@ -1491,7 +1548,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>14</v>
@@ -1514,7 +1571,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>14</v>
@@ -1534,7 +1591,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1559,7 +1616,7 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -1618,7 +1675,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>14</v>
@@ -1641,7 +1698,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>14</v>
@@ -1664,7 +1721,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>14</v>
@@ -1687,7 +1744,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>14</v>
@@ -1710,7 +1767,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>14</v>
@@ -1733,7 +1790,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>14</v>
@@ -1756,7 +1813,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>18</v>
@@ -1779,7 +1836,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>18</v>
@@ -1802,7 +1859,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>18</v>
@@ -1825,7 +1882,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>18</v>
@@ -1848,7 +1905,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>19</v>
@@ -1871,7 +1928,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>14</v>
@@ -1894,7 +1951,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>14</v>
@@ -1917,7 +1974,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>14</v>
@@ -1967,7 +2024,7 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2026,7 +2083,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>14</v>
@@ -2049,7 +2106,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>14</v>
@@ -2072,7 +2129,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>14</v>
@@ -2095,7 +2152,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>14</v>
@@ -2118,7 +2175,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>14</v>
@@ -2141,7 +2198,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>14</v>
@@ -2164,7 +2221,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>18</v>
@@ -2187,7 +2244,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>18</v>
@@ -2210,7 +2267,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>18</v>
@@ -2233,7 +2290,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>18</v>
@@ -2256,7 +2313,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>19</v>
@@ -2279,7 +2336,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>14</v>
@@ -2302,7 +2359,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>14</v>
@@ -2325,7 +2382,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>14</v>
@@ -2375,7 +2432,7 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -2434,7 +2491,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>14</v>
@@ -2446,7 +2503,7 @@
         <v>360</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>16</v>
@@ -2460,7 +2517,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>14</v>
@@ -2472,7 +2529,7 @@
         <v>360</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>16</v>
@@ -2486,7 +2543,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>14</v>
@@ -2498,7 +2555,7 @@
         <v>360</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>16</v>
@@ -2512,7 +2569,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>14</v>
@@ -2524,7 +2581,7 @@
         <v>360</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>16</v>
@@ -2538,7 +2595,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>14</v>
@@ -2550,13 +2607,13 @@
         <v>360</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2564,7 +2621,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>14</v>
@@ -2576,7 +2633,7 @@
         <v>30</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>16</v>
@@ -2590,7 +2647,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>18</v>
@@ -2602,7 +2659,7 @@
         <v>360</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>16</v>
@@ -2616,7 +2673,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>18</v>
@@ -2628,7 +2685,7 @@
         <v>360</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>16</v>
@@ -2642,7 +2699,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>18</v>
@@ -2654,7 +2711,7 @@
         <v>360</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>16</v>
@@ -2668,7 +2725,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>18</v>
@@ -2680,7 +2737,7 @@
         <v>30</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>16</v>
@@ -2694,7 +2751,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>19</v>
@@ -2706,7 +2763,7 @@
         <v>360</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>16</v>
@@ -2720,7 +2777,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>14</v>
@@ -2732,7 +2789,7 @@
         <v>360</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>20</v>
@@ -2746,7 +2803,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>14</v>
@@ -2758,7 +2815,7 @@
         <v>360</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>21</v>
@@ -2772,7 +2829,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>14</v>
@@ -2784,7 +2841,7 @@
         <v>360</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>22</v>
@@ -2795,7 +2852,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>